<commit_message>
Implemented the locked mpmc alt buffer and gathered data from it. There does not appear to be much difference between mpmc and its alt at first glance. Regathered perf data for linked list locked+lockless and for key range 128
</commit_message>
<xml_diff>
--- a/Data Structures/linked_list/MPMC_Buffer_Test_Data.xlsx
+++ b/Data Structures/linked_list/MPMC_Buffer_Test_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830"/>
+    <workbookView xWindow="240" yWindow="345" windowWidth="14805" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1379,11 +1379,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="58073088"/>
-        <c:axId val="58075392"/>
+        <c:axId val="39371904"/>
+        <c:axId val="39374208"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="58073088"/>
+        <c:axId val="39371904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1411,7 +1411,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58075392"/>
+        <c:crossAx val="39374208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1419,7 +1419,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="58075392"/>
+        <c:axId val="39374208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1448,7 +1448,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58073088"/>
+        <c:crossAx val="39371904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1677,11 +1677,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39111680"/>
-        <c:axId val="39113856"/>
+        <c:axId val="59198080"/>
+        <c:axId val="59204352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39111680"/>
+        <c:axId val="59198080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1709,7 +1709,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39113856"/>
+        <c:crossAx val="59204352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1717,7 +1717,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39113856"/>
+        <c:axId val="59204352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1746,7 +1746,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39111680"/>
+        <c:crossAx val="59198080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1975,11 +1975,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39599104"/>
-        <c:axId val="39601280"/>
+        <c:axId val="59222656"/>
+        <c:axId val="59233024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39599104"/>
+        <c:axId val="59222656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2007,7 +2007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39601280"/>
+        <c:crossAx val="59233024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2015,7 +2015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39601280"/>
+        <c:axId val="59233024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2044,7 +2044,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39599104"/>
+        <c:crossAx val="59222656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2103,6 +2103,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2562,11 +2563,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39641088"/>
-        <c:axId val="39643008"/>
+        <c:axId val="122183040"/>
+        <c:axId val="122283520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39641088"/>
+        <c:axId val="122183040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2588,13 +2589,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39643008"/>
+        <c:crossAx val="122283520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2602,7 +2604,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39643008"/>
+        <c:axId val="122283520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2625,19 +2627,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39641088"/>
+        <c:crossAx val="122183040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2687,6 +2691,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2999,11 +3004,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39663872"/>
-        <c:axId val="39678336"/>
+        <c:axId val="122464128"/>
+        <c:axId val="122523648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39663872"/>
+        <c:axId val="122464128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3025,13 +3030,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39678336"/>
+        <c:crossAx val="122523648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3039,7 +3045,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39678336"/>
+        <c:axId val="122523648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3062,19 +3068,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39663872"/>
+        <c:crossAx val="122464128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -3415,11 +3423,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39695104"/>
-        <c:axId val="39697024"/>
+        <c:axId val="123355520"/>
+        <c:axId val="123357440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39695104"/>
+        <c:axId val="123355520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3447,7 +3455,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39697024"/>
+        <c:crossAx val="123357440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3455,7 +3463,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39697024"/>
+        <c:axId val="123357440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3484,7 +3492,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39695104"/>
+        <c:crossAx val="123355520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3852,11 +3860,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39926784"/>
-        <c:axId val="39937152"/>
+        <c:axId val="123607680"/>
+        <c:axId val="59245312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39926784"/>
+        <c:axId val="123607680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3884,7 +3892,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39937152"/>
+        <c:crossAx val="59245312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3892,7 +3900,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39937152"/>
+        <c:axId val="59245312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3921,7 +3929,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39926784"/>
+        <c:crossAx val="123607680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4237,11 +4245,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39947264"/>
-        <c:axId val="39965824"/>
+        <c:axId val="59267712"/>
+        <c:axId val="59269888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39947264"/>
+        <c:axId val="59267712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4270,7 +4278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39965824"/>
+        <c:crossAx val="59269888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4278,7 +4286,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39965824"/>
+        <c:axId val="59269888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4308,7 +4316,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39947264"/>
+        <c:crossAx val="59267712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4360,6 +4368,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -4624,11 +4633,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39988224"/>
-        <c:axId val="39994496"/>
+        <c:axId val="59296384"/>
+        <c:axId val="59302656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39988224"/>
+        <c:axId val="59296384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4650,13 +4659,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39994496"/>
+        <c:crossAx val="59302656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4664,7 +4674,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39994496"/>
+        <c:axId val="59302656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4687,19 +4697,21 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39988224"/>
+        <c:crossAx val="59296384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -5009,11 +5021,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40016896"/>
-        <c:axId val="40019072"/>
+        <c:axId val="59386496"/>
+        <c:axId val="59405056"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40016896"/>
+        <c:axId val="59386496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5042,7 +5054,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40019072"/>
+        <c:crossAx val="59405056"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5050,7 +5062,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40019072"/>
+        <c:axId val="59405056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5080,7 +5092,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40016896"/>
+        <c:crossAx val="59386496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5889,11 +5901,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40067072"/>
-        <c:axId val="40068992"/>
+        <c:axId val="59448704"/>
+        <c:axId val="59459072"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40067072"/>
+        <c:axId val="59448704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5922,7 +5934,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40068992"/>
+        <c:crossAx val="59459072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5930,7 +5942,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40068992"/>
+        <c:axId val="59459072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5960,7 +5972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40067072"/>
+        <c:crossAx val="59448704"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7014,11 +7026,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="112785280"/>
-        <c:axId val="114274688"/>
+        <c:axId val="40296832"/>
+        <c:axId val="40322176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="112785280"/>
+        <c:axId val="40296832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7046,7 +7058,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="114274688"/>
+        <c:crossAx val="40322176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7054,7 +7066,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="114274688"/>
+        <c:axId val="40322176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7083,7 +7095,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="112785280"/>
+        <c:crossAx val="40296832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8062,11 +8074,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40107008"/>
-        <c:axId val="40121472"/>
+        <c:axId val="59505280"/>
+        <c:axId val="59581184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40107008"/>
+        <c:axId val="59505280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8095,7 +8107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40121472"/>
+        <c:crossAx val="59581184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8103,7 +8115,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40121472"/>
+        <c:axId val="59581184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8133,7 +8145,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40107008"/>
+        <c:crossAx val="59505280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -9100,11 +9112,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40158720"/>
-        <c:axId val="40160640"/>
+        <c:axId val="59626624"/>
+        <c:axId val="59628544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40158720"/>
+        <c:axId val="59626624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9133,7 +9145,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40160640"/>
+        <c:crossAx val="59628544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -9141,7 +9153,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40160640"/>
+        <c:axId val="59628544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9171,7 +9183,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40158720"/>
+        <c:crossAx val="59626624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10151,11 +10163,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40230912"/>
-        <c:axId val="40232832"/>
+        <c:axId val="59669888"/>
+        <c:axId val="59680256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40230912"/>
+        <c:axId val="59669888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10183,7 +10195,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40232832"/>
+        <c:crossAx val="59680256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10191,7 +10203,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40232832"/>
+        <c:axId val="59680256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10220,7 +10232,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40230912"/>
+        <c:crossAx val="59669888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10550,11 +10562,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40583168"/>
-        <c:axId val="40585088"/>
+        <c:axId val="59719040"/>
+        <c:axId val="59721216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40583168"/>
+        <c:axId val="59719040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10582,7 +10594,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40585088"/>
+        <c:crossAx val="59721216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10590,7 +10602,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40585088"/>
+        <c:axId val="59721216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10619,7 +10631,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40583168"/>
+        <c:crossAx val="59719040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10939,11 +10951,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40598912"/>
-        <c:axId val="40613376"/>
+        <c:axId val="59751424"/>
+        <c:axId val="59753600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40598912"/>
+        <c:axId val="59751424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10971,7 +10983,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40613376"/>
+        <c:crossAx val="59753600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10979,7 +10991,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40613376"/>
+        <c:axId val="59753600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11008,7 +11020,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40598912"/>
+        <c:crossAx val="59751424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11328,11 +11340,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40701312"/>
-        <c:axId val="40707584"/>
+        <c:axId val="59841536"/>
+        <c:axId val="59864192"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40701312"/>
+        <c:axId val="59841536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11360,7 +11372,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40707584"/>
+        <c:crossAx val="59864192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11368,7 +11380,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40707584"/>
+        <c:axId val="59864192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11397,7 +11409,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40701312"/>
+        <c:crossAx val="59841536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11717,11 +11729,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="40717696"/>
-        <c:axId val="40732160"/>
+        <c:axId val="59890688"/>
+        <c:axId val="59892864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="40717696"/>
+        <c:axId val="59890688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11749,7 +11761,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40732160"/>
+        <c:crossAx val="59892864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -11757,7 +11769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="40732160"/>
+        <c:axId val="59892864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -11786,7 +11798,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="40717696"/>
+        <c:crossAx val="59890688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12826,11 +12838,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="117586944"/>
-        <c:axId val="117761536"/>
+        <c:axId val="42929536"/>
+        <c:axId val="43108992"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="117586944"/>
+        <c:axId val="42929536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12858,7 +12870,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117761536"/>
+        <c:crossAx val="43108992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -12866,7 +12878,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="117761536"/>
+        <c:axId val="43108992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12895,7 +12907,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="117586944"/>
+        <c:crossAx val="42929536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13129,11 +13141,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="38456704"/>
-        <c:axId val="38458880"/>
+        <c:axId val="108862848"/>
+        <c:axId val="120002048"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38456704"/>
+        <c:axId val="108862848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13161,7 +13173,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38458880"/>
+        <c:crossAx val="120002048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13169,7 +13181,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="38458880"/>
+        <c:axId val="120002048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13198,7 +13210,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38456704"/>
+        <c:crossAx val="108862848"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13427,11 +13439,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="38997376"/>
-        <c:axId val="39007744"/>
+        <c:axId val="121684736"/>
+        <c:axId val="121729024"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="38997376"/>
+        <c:axId val="121684736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13459,7 +13471,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39007744"/>
+        <c:crossAx val="121729024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13467,7 +13479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39007744"/>
+        <c:axId val="121729024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13496,7 +13508,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38997376"/>
+        <c:crossAx val="121684736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -13725,11 +13737,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39022592"/>
-        <c:axId val="39024512"/>
+        <c:axId val="122375168"/>
+        <c:axId val="122590336"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39022592"/>
+        <c:axId val="122375168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13757,7 +13769,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39024512"/>
+        <c:crossAx val="122590336"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -13765,7 +13777,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39024512"/>
+        <c:axId val="122590336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -13794,7 +13806,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39022592"/>
+        <c:crossAx val="122375168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14023,11 +14035,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39051264"/>
-        <c:axId val="39053184"/>
+        <c:axId val="123409920"/>
+        <c:axId val="123411840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39051264"/>
+        <c:axId val="123409920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14055,7 +14067,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39053184"/>
+        <c:crossAx val="123411840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14063,7 +14075,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39053184"/>
+        <c:axId val="123411840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14092,7 +14104,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39051264"/>
+        <c:crossAx val="123409920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14321,11 +14333,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39067008"/>
-        <c:axId val="39073280"/>
+        <c:axId val="43080320"/>
+        <c:axId val="43090688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39067008"/>
+        <c:axId val="43080320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14353,7 +14365,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39073280"/>
+        <c:crossAx val="43090688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14361,7 +14373,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39073280"/>
+        <c:axId val="43090688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14390,7 +14402,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39067008"/>
+        <c:crossAx val="43080320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -14598,11 +14610,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="39083008"/>
-        <c:axId val="39097472"/>
+        <c:axId val="43145856"/>
+        <c:axId val="59179776"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="39083008"/>
+        <c:axId val="43145856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14630,7 +14642,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39097472"/>
+        <c:crossAx val="59179776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -14638,7 +14650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39097472"/>
+        <c:axId val="59179776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -14667,7 +14679,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39083008"/>
+        <c:crossAx val="43145856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -15808,7 +15820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:O398"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
       <selection activeCell="H235" sqref="H235"/>
     </sheetView>
   </sheetViews>

</xml_diff>